<commit_message>
only changes in prediction_files
</commit_message>
<xml_diff>
--- a/scripts/prediction_files/config_predictions_files.xlsx
+++ b/scripts/prediction_files/config_predictions_files.xlsx
@@ -1,33 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProtoQSAR\COMPIS\ONTOX_2022\ONTOX_2022_T3.1\MANUSCRIPT\first_final_version\Processing_datasets\prediction_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\IRB\scripts\prediction_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3E5D47-63A9-47BB-99EC-B51A4A67CCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BD3BE1-5BD0-4661-A1ED-322877ED96D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7606FAE2-3BC8-44FB-90E7-845E574CC87B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7606FAE2-3BC8-44FB-90E7-845E574CC87B}"/>
   </bookViews>
   <sheets>
     <sheet name="input_files" sheetId="1" r:id="rId1"/>
     <sheet name="input_files_reserva" sheetId="3" r:id="rId2"/>
     <sheet name="help" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="99">
   <si>
     <t>CAS</t>
   </si>
@@ -650,9 +661,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -690,7 +701,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -796,7 +807,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -938,7 +949,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -948,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDD012A-314B-482D-B6D6-01F082109B2D}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1294,12 @@
       <c r="C9" s="8">
         <v>45553</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1394,12 +1410,7 @@
       <c r="C12" s="8">
         <v>45558</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1608,6 +1619,22 @@
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="11"/>
+      <c r="C18" s="8"/>
+      <c r="K18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N18" t="s">
+        <v>8</v>
+      </c>
+      <c r="O18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1699,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499EE394-536D-4EC2-B502-E60B4FC24917}">
   <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,7 +2223,9 @@
       <c r="C9" s="8">
         <v>45553</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="7" t="s">
         <v>24</v>
       </c>
@@ -2230,7 +2259,9 @@
       <c r="X9" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="Y9" s="21"/>
+      <c r="Y9" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="Z9" s="21"/>
       <c r="AA9" s="21"/>
       <c r="AB9" s="21"/>

</xml_diff>

<commit_message>
mas cambios en prediction files
</commit_message>
<xml_diff>
--- a/scripts/prediction_files/config_predictions_files.xlsx
+++ b/scripts/prediction_files/config_predictions_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\IRB\scripts\prediction_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BD3D4D-2122-436C-992F-102900ECF5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61FACBA-63AC-4EBC-9F42-0E5BB0CAF939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7606FAE2-3BC8-44FB-90E7-845E574CC87B}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="27000" windowHeight="14040" xr2:uid="{7606FAE2-3BC8-44FB-90E7-845E574CC87B}"/>
   </bookViews>
   <sheets>
     <sheet name="input_files" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="103">
   <si>
     <t>CAS</t>
   </si>
@@ -592,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -663,9 +663,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDD012A-314B-482D-B6D6-01F082109B2D}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,12 +1316,7 @@
       <c r="C9" s="8">
         <v>45553</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1655,13 +1649,13 @@
       <c r="E18" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="34"/>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="32"/>
       <c r="K18" t="s">
         <v>8</v>
       </c>
@@ -1681,6 +1675,22 @@
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="11"/>
+      <c r="I19" s="33"/>
+      <c r="K19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" t="s">
+        <v>48</v>
+      </c>
+      <c r="N19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O19" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1761,6 +1771,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>